<commit_message>
agregamos el horario de los tallers
</commit_message>
<xml_diff>
--- a/5_semestre/horario.xlsx
+++ b/5_semestre/horario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\A-U\5_semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Documentos\A-U\5_semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272DB1FC-81EB-44CD-8B82-D1BB32C20B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C67C9D7-A6DB-4CC1-8762-70AADA0C3580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Lunes</t>
   </si>
@@ -113,6 +113,15 @@
   <si>
     <t>Estructura 
 discreta</t>
+  </si>
+  <si>
+    <t>Taller</t>
+  </si>
+  <si>
+    <t>Talleres 15:00</t>
+  </si>
+  <si>
+    <t>Talleres 17:00</t>
   </si>
 </sst>
 </file>
@@ -128,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,6 +238,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -566,7 +587,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +698,9 @@
         <v>22</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="12" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -693,7 +716,9 @@
       <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -711,7 +736,9 @@
       <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
actualizamos todo el quinto semestre hasta la semana libre
</commit_message>
<xml_diff>
--- a/5_semestre/horario.xlsx
+++ b/5_semestre/horario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Documentos\A-U\5_semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\A-U\5_semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C67C9D7-A6DB-4CC1-8762-70AADA0C3580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5DA663-8AE3-4AD0-B3BD-F676BD0E3B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Lunes</t>
   </si>
@@ -122,6 +122,10 @@
   </si>
   <si>
     <t>Talleres 17:00</t>
+  </si>
+  <si>
+    <t>Ayudantia
+estructura</t>
   </si>
 </sst>
 </file>
@@ -587,7 +591,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +710,9 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="C8" s="6" t="s">
         <v>19</v>
       </c>

</xml_diff>